<commit_message>
Player stats updating over time
</commit_message>
<xml_diff>
--- a/Assets/Editor/Data/gd.xlsx
+++ b/Assets/Editor/Data/gd.xlsx
@@ -28998,10 +28998,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed some player formulas. Added cheats: T - time speed up; K - hit all player's health parts
</commit_message>
<xml_diff>
--- a/Assets/Editor/Data/gd.xlsx
+++ b/Assets/Editor/Data/gd.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -152,9 +152,6 @@
   </si>
   <si>
     <t>healthRegenHungerStage4</t>
-  </si>
-  <si>
-    <t>-0.1</t>
   </si>
   <si>
     <t>healthRegenThirstStage1</t>
@@ -29001,13 +28998,13 @@
       <c r="A23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>43</v>
+      <c r="B23" s="19">
+        <v>-5.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="17">
         <v>1.0</v>
@@ -29015,7 +29012,7 @@
     </row>
     <row r="25">
       <c r="A25" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>40</v>
@@ -29023,7 +29020,7 @@
     </row>
     <row r="26">
       <c r="A26" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>17</v>
@@ -29031,10 +29028,10 @@
     </row>
     <row r="27">
       <c r="A27" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>43</v>
+      <c r="B27" s="19">
+        <v>-5.0</v>
       </c>
     </row>
     <row r="28">
@@ -32946,30 +32943,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="20" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C2" s="3">
         <v>3.0</v>
@@ -32978,7 +32975,7 @@
         <v>120.0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="3">
         <v>3.0</v>
@@ -32986,10 +32983,10 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3">
         <v>2.0</v>
@@ -32998,7 +32995,7 @@
         <v>80.0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="3">
         <v>2.0</v>
@@ -33006,19 +33003,19 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="3">
         <v>60.0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="3">
         <v>4.0</v>
@@ -33026,10 +33023,10 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="21">
         <v>2.0</v>
@@ -33038,7 +33035,7 @@
         <v>50.0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" s="3">
         <v>4.0</v>
@@ -33050,7 +33047,7 @@
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6" s="3">
         <v>8.0</v>
@@ -33058,10 +33055,10 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="21">
         <v>1.0</v>
@@ -33070,7 +33067,7 @@
         <v>40.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="3">
         <v>2.0</v>
@@ -33082,7 +33079,7 @@
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F8" s="3">
         <v>4.0</v>
@@ -33090,10 +33087,10 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="3">
         <v>2.0</v>
@@ -33102,7 +33099,7 @@
         <v>40</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="3">
         <v>100.0</v>
@@ -41069,24 +41066,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="24">
         <v>1.0</v>
@@ -41106,7 +41103,7 @@
     </row>
     <row r="3">
       <c r="A3" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="24">
         <v>2.0</v>
@@ -41126,7 +41123,7 @@
     </row>
     <row r="4">
       <c r="A4" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="24">
         <v>1.0</v>
@@ -41146,7 +41143,7 @@
     </row>
     <row r="5">
       <c r="A5" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="24">
         <v>1.0</v>
@@ -41166,7 +41163,7 @@
     </row>
     <row r="6">
       <c r="A6" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="24">
         <v>1.0</v>
@@ -41186,7 +41183,7 @@
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="24">
         <v>1.0</v>
@@ -41206,7 +41203,7 @@
     </row>
     <row r="8">
       <c r="A8" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="24">
         <v>1.0</v>
@@ -41226,7 +41223,7 @@
     </row>
     <row r="9">
       <c r="A9" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="24">
         <v>1.0</v>
@@ -41246,7 +41243,7 @@
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="24">
         <v>1.0</v>
@@ -41266,7 +41263,7 @@
     </row>
     <row r="11">
       <c r="A11" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="24">
         <v>1.0</v>
@@ -49195,15 +49192,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="24">
         <v>2.0</v>
@@ -49214,7 +49211,7 @@
     </row>
     <row r="3">
       <c r="A3" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="24">
         <v>1.0</v>
@@ -49225,7 +49222,7 @@
     </row>
     <row r="4">
       <c r="A4" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="24">
         <v>1.0</v>
@@ -49236,7 +49233,7 @@
     </row>
     <row r="5">
       <c r="A5" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="24">
         <v>1.0</v>
@@ -49247,7 +49244,7 @@
     </row>
     <row r="6">
       <c r="A6" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="24">
         <v>1.0</v>
@@ -49258,7 +49255,7 @@
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="24">
         <v>1.0</v>
@@ -54247,18 +54244,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="27">
         <v>1.0</v>

</xml_diff>

<commit_message>
Added biome parser and base view
</commit_message>
<xml_diff>
--- a/Assets/Editor/Data/gd.xlsx
+++ b/Assets/Editor/Data/gd.xlsx
@@ -67,10 +67,10 @@
 7.Влияние на температурный режим ночью от 60% до 0% таймера</t>
   </si>
   <si>
-    <t>TemperatureBiom</t>
+    <t>BiomTemperature</t>
   </si>
   <si>
-    <t>HungerThirst</t>
+    <t>AffectValue</t>
   </si>
   <si>
     <t>forest.biome</t>

</xml_diff>